<commit_message>
Some formatting changes in repsonse to feedback
</commit_message>
<xml_diff>
--- a/data/10_CSCExp.xlsx
+++ b/data/10_CSCExp.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="EverCINCLA" sheetId="1" r:id="rId1"/>
-    <sheet name="CIN_waffle" sheetId="2" r:id="rId2"/>
-    <sheet name="CSC_timing" sheetId="3" r:id="rId3"/>
+    <sheet name="CIN_waffle_sv" sheetId="2" r:id="rId2"/>
+    <sheet name="CIN_waffle_any" sheetId="3" r:id="rId3"/>
+    <sheet name="CSC_timing" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -3897,6 +3898,531 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>propany_count_CIN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>also_propany_count_CIN</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>propany_count_not_CIN</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>not_also_propany_count_CIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Birmingham</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>81</v>
+      </c>
+      <c r="F2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bradford</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>80</v>
+      </c>
+      <c r="F3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Haringey</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>81</v>
+      </c>
+      <c r="F4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Lambeth</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>63</v>
+      </c>
+      <c r="F5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>66</v>
+      </c>
+      <c r="F7">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Manchester</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="D8">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>57</v>
+      </c>
+      <c r="F8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Newham</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>67</v>
+      </c>
+      <c r="F9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sheffield</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>65</v>
+      </c>
+      <c r="F10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Southwark</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>84</v>
+      </c>
+      <c r="F11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Birmingham</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>81</v>
+      </c>
+      <c r="F12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Bradford</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>79</v>
+      </c>
+      <c r="F13">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Haringey</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>72</v>
+      </c>
+      <c r="F14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Lambeth</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <v>68</v>
+      </c>
+      <c r="F15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>39</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>61</v>
+      </c>
+      <c r="F17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Manchester</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>23</v>
+      </c>
+      <c r="E18">
+        <v>62</v>
+      </c>
+      <c r="F18">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Newham</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>67</v>
+      </c>
+      <c r="F19">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sheffield</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>66</v>
+      </c>
+      <c r="F20">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Southwark</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>83</v>
+      </c>
+      <c r="F21">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E181"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>